<commit_message>
Subindo documentação, atualização do backlog, atualização dos slides
</commit_message>
<xml_diff>
--- a/Documentos/Excel/backlog-grupo3.xlsx
+++ b/Documentos/Excel/backlog-grupo3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25108"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B738745B-FC95-4B70-B0E8-E72996AD1F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{00BDC65B-34E6-4948-B49E-340E3EF7B524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Desejável, importante, essencial</t>
   </si>
@@ -65,13 +65,22 @@
   </si>
   <si>
     <t>Cliente Linux</t>
+  </si>
+  <si>
+    <t>Tela de Cadastro</t>
+  </si>
+  <si>
+    <t>Tela de login</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,18 +94,29 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <b/>
-      <sz val="9"/>
+      <sz val="9.5"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +153,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE4D6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -198,15 +224,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -218,40 +262,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -576,7 +611,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="D15" sqref="D15:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -610,7 +645,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" ht="16.5">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -631,14 +666,14 @@
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="6"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="7" t="s">
@@ -646,16 +681,16 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:9" ht="16.5">
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
@@ -676,14 +711,14 @@
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="15"/>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="6"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="16" t="s">
@@ -691,14 +726,14 @@
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="18"/>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="6"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="13" t="s">
@@ -706,14 +741,14 @@
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="6"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="13" t="s">
@@ -721,14 +756,14 @@
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="15"/>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="6"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="16" t="s">
@@ -736,113 +771,125 @@
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="6"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6"/>
+      <c r="A12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="6"/>
+      <c r="A13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="6"/>
+      <c r="A14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="12"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="6"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="12"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="6"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="12"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="6"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="12"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="6"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="38">
@@ -859,18 +906,12 @@
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="D11:I11"/>
-    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D20:I20"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="D16:I16"/>
     <mergeCell ref="D17:I17"/>
     <mergeCell ref="D5:I5"/>
     <mergeCell ref="D6:I6"/>
-    <mergeCell ref="D20:I20"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
     <mergeCell ref="D7:I7"/>
     <mergeCell ref="D8:I8"/>
     <mergeCell ref="D12:I12"/>
@@ -879,11 +920,17 @@
     <mergeCell ref="D15:I15"/>
     <mergeCell ref="D9:I9"/>
     <mergeCell ref="D10:I10"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="D1:I2"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D4:I4"/>
+    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>